<commit_message>
record model add apply member field
</commit_message>
<xml_diff>
--- a/systemFile/template_record.xlsx
+++ b/systemFile/template_record.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,14 @@
   </si>
   <si>
     <t>類別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申請人數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申請人數</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -164,7 +172,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -203,6 +211,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,11 +498,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -500,14 +509,15 @@
     <col min="3" max="3" width="10" style="6" customWidth="1"/>
     <col min="4" max="4" width="9" style="6"/>
     <col min="5" max="5" width="10.75" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9" style="6"/>
-    <col min="7" max="7" width="17.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18" style="6" customWidth="1"/>
-    <col min="9" max="10" width="14" style="6" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9" style="13"/>
+    <col min="7" max="7" width="9" style="6"/>
+    <col min="8" max="8" width="17.875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18" style="6" customWidth="1"/>
+    <col min="10" max="11" width="14" style="6" customWidth="1"/>
+    <col min="12" max="12" width="15.625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -520,9 +530,10 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -535,9 +546,10 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -550,9 +562,10 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
@@ -569,21 +582,24 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -595,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:K1048576"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -606,25 +622,28 @@
     <col min="1" max="1" width="9.75" style="10" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="10" customWidth="1"/>
     <col min="3" max="3" width="8.875" style="10" customWidth="1"/>
-    <col min="4" max="6" width="9" style="10"/>
-    <col min="7" max="7" width="16.375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="16.625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.25" style="10" customWidth="1"/>
-    <col min="10" max="10" width="10.625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.25" style="10" customWidth="1"/>
+    <col min="4" max="5" width="9" style="10"/>
+    <col min="6" max="6" width="9" style="13"/>
+    <col min="7" max="7" width="9" style="10"/>
+    <col min="8" max="8" width="16.375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="10.25" style="10" customWidth="1"/>
+    <col min="11" max="11" width="10.625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.25" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -641,27 +660,30 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>